<commit_message>
fill in NAs & rerun the data cleaning
</commit_message>
<xml_diff>
--- a/data/sim_res_fac.xlsx
+++ b/data/sim_res_fac.xlsx
@@ -707,12 +707,12 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>162.0</t>
+          <t>162</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -722,7 +722,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>100.0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -752,7 +752,7 @@
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>11.0</t>
+          <t>11</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
@@ -955,12 +955,12 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>12.0</t>
+          <t>12</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
@@ -970,7 +970,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>100.0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -978,9 +978,19 @@
           <t>no</t>
         </is>
       </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>23.0</t>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
@@ -990,7 +1000,7 @@
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
@@ -1133,7 +1143,8 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1037/met0000386_x000D_</t>
+          <t xml:space="preserve">https://doi.org/10.1037/met0000386_x000D_
+</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1183,12 +1194,12 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>15.0</t>
+          <t>15</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -1198,7 +1209,7 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>1000.0</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -1216,6 +1227,11 @@
           <t>1?</t>
         </is>
       </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="X4" t="inlineStr">
         <is>
           <t>known</t>
@@ -1223,7 +1239,7 @@
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
@@ -1353,7 +1369,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>8</t>
         </is>
       </c>
       <c r="B5">
@@ -1411,12 +1427,12 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>135.0</t>
+          <t>135</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
@@ -1426,7 +1442,7 @@
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>5000.0</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
@@ -1441,7 +1457,7 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
@@ -1456,7 +1472,7 @@
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
@@ -1586,7 +1602,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B6">
@@ -1644,12 +1660,12 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
@@ -1659,7 +1675,7 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>100.0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -1674,7 +1690,7 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>8</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
@@ -1689,7 +1705,7 @@
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
@@ -1809,7 +1825,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>11.0</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B7">
@@ -1872,12 +1888,12 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>9</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -1887,7 +1903,7 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>10000.0</t>
+          <t>10000</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -1902,7 +1918,7 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
@@ -1917,7 +1933,7 @@
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="Z7" t="inlineStr">
@@ -2042,7 +2058,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>11.0</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B8">
@@ -2120,7 +2136,7 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>1000.0</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -2135,7 +2151,7 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>8</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
@@ -2270,7 +2286,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>12.0</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B9">
@@ -2328,12 +2344,12 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>30.0</t>
+          <t>30</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
@@ -2343,7 +2359,7 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>500.0</t>
+          <t>500</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -2373,7 +2389,7 @@
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Z9" t="inlineStr">
@@ -2498,7 +2514,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B10">
@@ -2551,12 +2567,12 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>216.0</t>
+          <t>216</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -2566,7 +2582,7 @@
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>1000.0</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
@@ -2596,7 +2612,7 @@
       </c>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="Z10" t="inlineStr">
@@ -2726,7 +2742,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>14.0</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B11">
@@ -2784,12 +2800,12 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>18.0</t>
+          <t>18</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
@@ -2799,7 +2815,7 @@
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>1000.0</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
@@ -2829,7 +2845,7 @@
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Z11" t="inlineStr">
@@ -2959,7 +2975,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>15.0</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B12">
@@ -3017,12 +3033,12 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
@@ -3062,7 +3078,7 @@
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="Z12" t="inlineStr">
@@ -3197,7 +3213,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>16.0</t>
+          <t>16</t>
         </is>
       </c>
       <c r="B13">
@@ -3255,12 +3271,12 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
@@ -3270,7 +3286,7 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>10000.0</t>
+          <t>10000</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
@@ -3285,7 +3301,7 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
@@ -3300,7 +3316,7 @@
       </c>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Z13" t="inlineStr">
@@ -3430,7 +3446,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>17.0</t>
+          <t>17</t>
         </is>
       </c>
       <c r="B14">
@@ -3493,12 +3509,12 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>360.0</t>
+          <t>360</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
@@ -3508,7 +3524,7 @@
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>3000.0</t>
+          <t>3000</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
@@ -3538,7 +3554,7 @@
       </c>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Z14" t="inlineStr">
@@ -3663,7 +3679,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>18.0</t>
+          <t>18</t>
         </is>
       </c>
       <c r="B15">
@@ -3721,12 +3737,12 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
@@ -3736,7 +3752,7 @@
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>400.0</t>
+          <t>400</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
@@ -3766,7 +3782,7 @@
       </c>
       <c r="Y15" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Z15" t="inlineStr">
@@ -3896,7 +3912,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>19.0</t>
+          <t>19</t>
         </is>
       </c>
       <c r="B16">
@@ -3954,12 +3970,12 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
@@ -3969,7 +3985,7 @@
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>500.0</t>
+          <t>500</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
@@ -3984,7 +4000,7 @@
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>11.0</t>
+          <t>11</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
@@ -3999,7 +4015,7 @@
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Z16" t="inlineStr">
@@ -4119,7 +4135,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20.0</t>
+          <t>20</t>
         </is>
       </c>
       <c r="B17">
@@ -4182,12 +4198,12 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>24.0</t>
+          <t>24</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
@@ -4197,7 +4213,7 @@
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>100.0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
@@ -4212,7 +4228,7 @@
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>37.0</t>
+          <t>37</t>
         </is>
       </c>
       <c r="W17" t="inlineStr">
@@ -4227,7 +4243,7 @@
       </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Z17" t="inlineStr">
@@ -4357,7 +4373,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>22.0</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B18">
@@ -4420,12 +4436,12 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>135.0</t>
+          <t>135</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
@@ -4435,7 +4451,7 @@
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>1000.0</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
@@ -4465,7 +4481,7 @@
       </c>
       <c r="Y18" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Z18" t="inlineStr">
@@ -4595,7 +4611,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>23.0</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B19">
@@ -4653,12 +4669,12 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>16.0</t>
+          <t>16</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
@@ -4668,7 +4684,7 @@
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>2000.0</t>
+          <t>2000</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
@@ -4683,7 +4699,7 @@
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>7</t>
         </is>
       </c>
       <c r="W19" t="inlineStr">
@@ -4698,7 +4714,7 @@
       </c>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Z19" t="inlineStr">
@@ -4823,7 +4839,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>25.0</t>
+          <t>25</t>
         </is>
       </c>
       <c r="B20">
@@ -4881,12 +4897,12 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>72.0</t>
+          <t>72</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
@@ -4896,7 +4912,7 @@
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>800.0</t>
+          <t>800</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
@@ -4911,7 +4927,7 @@
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
@@ -4926,7 +4942,7 @@
       </c>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>7</t>
         </is>
       </c>
       <c r="Z20" t="inlineStr">
@@ -5056,7 +5072,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>29.0</t>
+          <t>29</t>
         </is>
       </c>
       <c r="B21">
@@ -5119,12 +5135,12 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>32.0</t>
+          <t>32</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
@@ -5134,7 +5150,7 @@
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>1000.0</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
@@ -5149,7 +5165,7 @@
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
@@ -5164,7 +5180,7 @@
       </c>
       <c r="Y21" t="inlineStr">
         <is>
-          <t>11.0</t>
+          <t>11</t>
         </is>
       </c>
       <c r="Z21" t="inlineStr">
@@ -5294,7 +5310,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>32.0</t>
+          <t>32</t>
         </is>
       </c>
       <c r="B22">
@@ -5352,12 +5368,12 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>90.0</t>
+          <t>90</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>7</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
@@ -5367,7 +5383,7 @@
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>2000.0</t>
+          <t>2000</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
@@ -5382,7 +5398,7 @@
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
@@ -5397,7 +5413,7 @@
       </c>
       <c r="Y22" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="Z22" t="inlineStr">
@@ -5532,7 +5548,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>38.0</t>
+          <t>38</t>
         </is>
       </c>
       <c r="B23">
@@ -5590,12 +5606,12 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>48.0</t>
+          <t>48</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
@@ -5605,7 +5621,7 @@
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>500.0</t>
+          <t>500</t>
         </is>
       </c>
       <c r="S23" t="inlineStr">
@@ -5635,7 +5651,7 @@
       </c>
       <c r="Y23" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="Z23" t="inlineStr">
@@ -5765,7 +5781,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>50.0</t>
+          <t>50</t>
         </is>
       </c>
       <c r="B24">
@@ -5823,12 +5839,12 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>16.0</t>
+          <t>16</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
@@ -5838,7 +5854,7 @@
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>1000.0</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="S24" t="inlineStr">
@@ -5853,7 +5869,7 @@
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="W24" t="inlineStr">
@@ -5868,7 +5884,7 @@
       </c>
       <c r="Y24" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Z24" t="inlineStr">
@@ -6003,7 +6019,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>55.0</t>
+          <t>55</t>
         </is>
       </c>
       <c r="B25">
@@ -6066,12 +6082,12 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>10</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
@@ -6081,7 +6097,7 @@
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>100.0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="S25" t="inlineStr">
@@ -6096,7 +6112,7 @@
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>30.0</t>
+          <t>30</t>
         </is>
       </c>
       <c r="W25" t="inlineStr">
@@ -6111,7 +6127,7 @@
       </c>
       <c r="Y25" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>9</t>
         </is>
       </c>
       <c r="Z25" t="inlineStr">
@@ -6246,7 +6262,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>56.0</t>
+          <t>56</t>
         </is>
       </c>
       <c r="B26">
@@ -6309,12 +6325,12 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>72.0</t>
+          <t>72</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
@@ -6324,7 +6340,7 @@
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>1000.0</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="S26" t="inlineStr">
@@ -6354,7 +6370,7 @@
       </c>
       <c r="Y26" t="inlineStr">
         <is>
-          <t>11.0</t>
+          <t>11</t>
         </is>
       </c>
       <c r="Z26" t="inlineStr">
@@ -6479,7 +6495,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>57.0</t>
+          <t>57</t>
         </is>
       </c>
       <c r="B27">
@@ -6542,12 +6558,12 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
@@ -6557,7 +6573,7 @@
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>1000.0</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="S27" t="inlineStr">
@@ -6587,7 +6603,7 @@
       </c>
       <c r="Y27" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Z27" t="inlineStr">
@@ -6717,7 +6733,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>58.0</t>
+          <t>58</t>
         </is>
       </c>
       <c r="B28">
@@ -6780,12 +6796,12 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>72.0</t>
+          <t>72</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
@@ -6795,7 +6811,7 @@
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>5000.0</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
@@ -6810,7 +6826,7 @@
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="W28" t="inlineStr">
@@ -6825,7 +6841,7 @@
       </c>
       <c r="Y28" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="Z28" t="inlineStr">
@@ -6960,7 +6976,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>62.0</t>
+          <t>62</t>
         </is>
       </c>
       <c r="B29">
@@ -7023,12 +7039,12 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>48.0</t>
+          <t>48</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
@@ -7038,7 +7054,7 @@
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>1000.0</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="S29" t="inlineStr">
@@ -7053,7 +7069,7 @@
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>13</t>
         </is>
       </c>
       <c r="W29" t="inlineStr">
@@ -7068,7 +7084,7 @@
       </c>
       <c r="Y29" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Z29" t="inlineStr">
@@ -7193,7 +7209,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>64.0</t>
+          <t>64</t>
         </is>
       </c>
       <c r="B30">
@@ -7246,12 +7262,12 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
@@ -7261,7 +7277,7 @@
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>1000.0</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
@@ -7276,7 +7292,7 @@
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="W30" t="inlineStr">
@@ -7291,7 +7307,7 @@
       </c>
       <c r="Y30" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>10</t>
         </is>
       </c>
       <c r="Z30" t="inlineStr">
@@ -7416,7 +7432,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>65.0</t>
+          <t>65</t>
         </is>
       </c>
       <c r="B31">
@@ -7474,7 +7490,7 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
@@ -7484,7 +7500,7 @@
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
@@ -7524,7 +7540,7 @@
       </c>
       <c r="Y31" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Z31" t="inlineStr">
@@ -7649,7 +7665,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>73.0</t>
+          <t>73</t>
         </is>
       </c>
       <c r="B32">
@@ -7707,12 +7723,12 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>1344.0</t>
+          <t>1344</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
@@ -7722,7 +7738,7 @@
       </c>
       <c r="R32" t="inlineStr">
         <is>
-          <t>5000.0</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="S32" t="inlineStr">
@@ -7742,7 +7758,7 @@
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="W32" t="inlineStr">
@@ -7882,7 +7898,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>74.0</t>
+          <t>74</t>
         </is>
       </c>
       <c r="B33">
@@ -7940,12 +7956,12 @@
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
@@ -7955,7 +7971,7 @@
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>5000.0</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="S33" t="inlineStr">
@@ -7985,7 +8001,7 @@
       </c>
       <c r="Y33" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Z33" t="inlineStr">
@@ -8120,7 +8136,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>77.0</t>
+          <t>77</t>
         </is>
       </c>
       <c r="B34">
@@ -8183,12 +8199,12 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr">
@@ -8198,7 +8214,7 @@
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>200.0</t>
+          <t>200</t>
         </is>
       </c>
       <c r="S34" t="inlineStr">
@@ -8228,7 +8244,7 @@
       </c>
       <c r="Y34" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Z34" t="inlineStr">
@@ -8348,7 +8364,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>78.0</t>
+          <t>78</t>
         </is>
       </c>
       <c r="B35">
@@ -8406,12 +8422,12 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>216.0</t>
+          <t>216</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
@@ -8421,7 +8437,7 @@
       </c>
       <c r="R35" t="inlineStr">
         <is>
-          <t>500.0</t>
+          <t>500</t>
         </is>
       </c>
       <c r="S35" t="inlineStr">
@@ -8451,7 +8467,7 @@
       </c>
       <c r="Y35" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>13</t>
         </is>
       </c>
       <c r="Z35" t="inlineStr">

</xml_diff>

<commit_message>
fix recoding bug in "issue" col
</commit_message>
<xml_diff>
--- a/data/sim_res_fac.xlsx
+++ b/data/sim_res_fac.xlsx
@@ -5194,7 +5194,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -5234,7 +5234,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -5477,7 +5477,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -5517,7 +5517,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -5597,7 +5597,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -5840,7 +5840,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -5880,7 +5880,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -5920,7 +5920,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -6163,7 +6163,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -6203,7 +6203,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -6243,7 +6243,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -6283,7 +6283,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -6323,7 +6323,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -6363,7 +6363,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -6601,7 +6601,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -6641,7 +6641,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -6681,7 +6681,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -6721,7 +6721,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -6761,7 +6761,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -6801,7 +6801,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -6841,7 +6841,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -6881,7 +6881,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -6921,7 +6921,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -6961,7 +6961,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -7001,7 +7001,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -7041,7 +7041,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -7284,7 +7284,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -7324,7 +7324,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -7364,7 +7364,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -7404,7 +7404,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -7444,7 +7444,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -7692,7 +7692,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -7930,7 +7930,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -8173,7 +8173,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -8421,7 +8421,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -8461,7 +8461,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -8501,7 +8501,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -8541,7 +8541,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -8779,7 +8779,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -9565,7 +9565,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -9803,7 +9803,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -10046,7 +10046,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -10087,7 +10087,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -10127,7 +10127,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -10360,7 +10360,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -10593,7 +10593,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -10633,7 +10633,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -11109,7 +11109,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -11352,7 +11352,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -11590,7 +11590,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -11833,7 +11833,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -13258,7 +13258,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -13506,7 +13506,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -13764,7 +13764,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -14017,7 +14017,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -14290,7 +14290,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -14330,7 +14330,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -14370,7 +14370,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -14410,7 +14410,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -14450,7 +14450,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -14713,7 +14713,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -14753,7 +14753,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -15006,7 +15006,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -15259,7 +15259,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -15512,7 +15512,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -15552,7 +15552,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -15597,7 +15597,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -15860,7 +15860,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -15905,7 +15905,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -15945,7 +15945,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -15990,7 +15990,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -16248,7 +16248,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -16288,7 +16288,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -16328,7 +16328,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -16368,7 +16368,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -16408,7 +16408,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -16448,7 +16448,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -16488,7 +16488,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -16528,7 +16528,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -16568,7 +16568,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -16608,7 +16608,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -16648,7 +16648,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -16688,7 +16688,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -16728,7 +16728,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -16991,7 +16991,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -17031,7 +17031,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -17071,7 +17071,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -17111,7 +17111,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -17151,7 +17151,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -17191,7 +17191,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -17231,7 +17231,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -17271,7 +17271,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -17529,7 +17529,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -17569,7 +17569,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -17609,7 +17609,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -17649,7 +17649,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -17689,7 +17689,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -17942,7 +17942,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -17982,7 +17982,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -18245,7 +18245,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -18285,7 +18285,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -18538,7 +18538,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -18578,7 +18578,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -18623,7 +18623,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -18663,7 +18663,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -18708,7 +18708,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -18748,7 +18748,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -18788,7 +18788,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -18828,7 +18828,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -18868,7 +18868,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -18908,7 +18908,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -18948,7 +18948,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -19196,7 +19196,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -19241,7 +19241,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -19281,7 +19281,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -19321,7 +19321,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -19361,7 +19361,7 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -19401,7 +19401,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -19441,7 +19441,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -19481,7 +19481,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -19521,7 +19521,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -19561,7 +19561,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
@@ -19601,7 +19601,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -19641,7 +19641,7 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -19681,7 +19681,7 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -19949,7 +19949,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
@@ -20197,7 +20197,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -20237,7 +20237,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -20277,7 +20277,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -20317,7 +20317,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
@@ -20570,7 +20570,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
@@ -20843,7 +20843,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
@@ -21101,7 +21101,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
@@ -21359,7 +21359,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
@@ -21617,7 +21617,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -21880,7 +21880,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -22128,7 +22128,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
@@ -22381,7 +22381,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
@@ -22912,7 +22912,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
@@ -23433,7 +23433,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
@@ -23939,7 +23939,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
@@ -26851,7 +26851,7 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
@@ -27094,7 +27094,7 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
@@ -27332,7 +27332,7 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
@@ -27375,7 +27375,7 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
@@ -27418,7 +27418,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
@@ -27461,7 +27461,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
@@ -27504,7 +27504,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
@@ -27547,7 +27547,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
@@ -27590,7 +27590,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
@@ -27838,7 +27838,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
@@ -27881,7 +27881,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
@@ -27924,7 +27924,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
@@ -27967,7 +27967,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
@@ -28205,7 +28205,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
@@ -28248,7 +28248,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
@@ -28291,7 +28291,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
@@ -28334,7 +28334,7 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
@@ -28377,7 +28377,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
@@ -28420,7 +28420,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
@@ -28463,7 +28463,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
@@ -28506,7 +28506,7 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
@@ -28549,7 +28549,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
@@ -28592,7 +28592,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
@@ -28635,7 +28635,7 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
@@ -28883,7 +28883,7 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
@@ -28926,7 +28926,7 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
@@ -29179,7 +29179,7 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D248" t="inlineStr">
@@ -29222,7 +29222,7 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D249" t="inlineStr">
@@ -29265,7 +29265,7 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D250" t="inlineStr">
@@ -29308,7 +29308,7 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
@@ -29351,7 +29351,7 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D252" t="inlineStr">
@@ -29394,7 +29394,7 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D253" t="inlineStr">
@@ -29437,7 +29437,7 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D254" t="inlineStr">
@@ -29480,7 +29480,7 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D255" t="inlineStr">
@@ -29523,7 +29523,7 @@
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D256" t="inlineStr">
@@ -29566,7 +29566,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D257" t="inlineStr">
@@ -29609,7 +29609,7 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D258" t="inlineStr">
@@ -29652,7 +29652,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D259" t="inlineStr">
@@ -29885,7 +29885,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
@@ -30128,7 +30128,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D261" t="inlineStr">
@@ -30366,7 +30366,7 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D262" t="inlineStr">
@@ -30604,7 +30604,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D263" t="inlineStr">
@@ -30852,7 +30852,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D264" t="inlineStr">
@@ -31095,7 +31095,7 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D265" t="inlineStr">
@@ -31138,7 +31138,7 @@
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D266" t="inlineStr">
@@ -31371,7 +31371,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D267" t="inlineStr">
@@ -31414,7 +31414,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D268" t="inlineStr">
@@ -31647,7 +31647,7 @@
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D269" t="inlineStr">
@@ -31690,7 +31690,7 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
@@ -31733,7 +31733,7 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
@@ -31976,7 +31976,7 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D272" t="inlineStr">
@@ -32209,7 +32209,7 @@
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D273" t="inlineStr">
@@ -32447,7 +32447,7 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D274" t="inlineStr">
@@ -32490,7 +32490,7 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D275" t="inlineStr">
@@ -32728,7 +32728,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D276" t="inlineStr">
@@ -32966,7 +32966,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D277" t="inlineStr">
@@ -35188,7 +35188,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D306" t="inlineStr">
@@ -35231,7 +35231,7 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D307" t="inlineStr">
@@ -35274,7 +35274,7 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D308" t="inlineStr">
@@ -35317,7 +35317,7 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D309" t="inlineStr">
@@ -35360,7 +35360,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D310" t="inlineStr">
@@ -35598,7 +35598,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D311" t="inlineStr">
@@ -35641,7 +35641,7 @@
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D312" t="inlineStr">
@@ -35684,7 +35684,7 @@
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D313" t="inlineStr">
@@ -35727,7 +35727,7 @@
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D314" t="inlineStr">
@@ -35770,7 +35770,7 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D315" t="inlineStr">
@@ -35813,7 +35813,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D316" t="inlineStr">
@@ -35856,7 +35856,7 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D317" t="inlineStr">
@@ -35899,7 +35899,7 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D318" t="inlineStr">
@@ -35942,7 +35942,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D319" t="inlineStr">
@@ -36185,7 +36185,7 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D320" t="inlineStr">
@@ -36228,7 +36228,7 @@
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D321" t="inlineStr">
@@ -36271,7 +36271,7 @@
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D322" t="inlineStr">
@@ -36314,7 +36314,7 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D323" t="inlineStr">
@@ -36552,7 +36552,7 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D324" t="inlineStr">
@@ -36595,7 +36595,7 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D325" t="inlineStr">
@@ -36638,7 +36638,7 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D326" t="inlineStr">
@@ -36681,7 +36681,7 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D327" t="inlineStr">
@@ -36724,7 +36724,7 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D328" t="inlineStr">
@@ -36767,7 +36767,7 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D329" t="inlineStr">
@@ -36810,7 +36810,7 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D330" t="inlineStr">
@@ -36853,7 +36853,7 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D331" t="inlineStr">
@@ -36896,7 +36896,7 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D332" t="inlineStr">
@@ -37139,7 +37139,7 @@
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D333" t="inlineStr">
@@ -37425,7 +37425,7 @@
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D335" t="inlineStr">
@@ -37668,7 +37668,7 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D336" t="inlineStr">

</xml_diff>

<commit_message>
redo analyses after NA addition
</commit_message>
<xml_diff>
--- a/data/sim_res_fac.xlsx
+++ b/data/sim_res_fac.xlsx
@@ -13416,6 +13416,11 @@
           <t>standard deviations</t>
         </is>
       </c>
+      <c r="AJ96" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
       <c r="AL96" t="inlineStr">
         <is>
           <t>nowhere</t>
@@ -32022,6 +32027,11 @@
       <c r="L272" t="inlineStr">
         <is>
           <t>parametric thin-air</t>
+        </is>
+      </c>
+      <c r="M272" t="inlineStr">
+        <is>
+          <t>yes</t>
         </is>
       </c>
       <c r="N272" t="inlineStr">

</xml_diff>

<commit_message>
udpate comp environment coding for two studies
we increased the rating after reviewer feedback, no change in overall results pattern
</commit_message>
<xml_diff>
--- a/data/sim_res_fac.xlsx
+++ b/data/sim_res_fac.xlsx
@@ -24771,7 +24771,7 @@
       </c>
       <c r="AX206" t="inlineStr">
         <is>
-          <t>minimal</t>
+          <t>partially</t>
         </is>
       </c>
       <c r="AY206" t="inlineStr">
@@ -34411,7 +34411,7 @@
       </c>
       <c r="AX310" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>partially</t>
         </is>
       </c>
       <c r="AY310" t="inlineStr">

</xml_diff>